<commit_message>
added 2-Sem/2.5.1/2_5_1_tex, 2_5_1.pdf, replaced 2_5_1.xlsx
</commit_message>
<xml_diff>
--- a/2-Sem/2.5.1/2_5_1.xlsx
+++ b/2-Sem/2.5.1/2_5_1.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vladislavchernienko/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vladislavchernienko/Desktop/Лабы/2.5.1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62DEAF77-8A96-7142-8DB8-3081E67AD1C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E62DBC8-C2E1-EE49-8046-4EF6CD8D6147}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{E5CFA479-68D7-2943-8B92-33F77FF5579D}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14020" xr2:uid="{E5CFA479-68D7-2943-8B92-33F77FF5579D}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -331,31 +331,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>348.33220799999998</c:v>
+                  <c:v>281.97492237599999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>346.37087799999995</c:v>
+                  <c:v>280.38722574100001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>344.40954799999997</c:v>
+                  <c:v>278.79952910599997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>343.23275000000001</c:v>
+                  <c:v>277.84691112500002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>342.05595199999999</c:v>
+                  <c:v>276.89429314400002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>339.31009</c:v>
+                  <c:v>274.67151785499999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>337.34876000000003</c:v>
+                  <c:v>273.08382122</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>336.17196200000001</c:v>
+                  <c:v>272.131203239</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>334.60289799999998</c:v>
+                  <c:v>270.86104593099998</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1487,7 +1487,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1536,12 +1536,12 @@
         <v>39</v>
       </c>
       <c r="B2" s="1">
-        <f>39*0.2*9.80665</f>
-        <v>76.491870000000006</v>
+        <f>0.039*0.2*9.80665*809.5</f>
+        <v>61.920168765</v>
       </c>
       <c r="C2" s="1">
         <f>22.75*10^-3 * 2 / B2 * 10^3 * 2</f>
-        <v>1.1896689151409163</v>
+        <v>1.4696342373575246</v>
       </c>
       <c r="D2" s="1">
         <v>1.2</v>
@@ -1550,8 +1550,8 @@
         <v>110</v>
       </c>
       <c r="F2" s="3">
-        <f>E2*0.2*9.80665</f>
-        <v>215.74629999999999</v>
+        <f>E2*0.2*9.80665*0.8095</f>
+        <v>174.64662984999998</v>
       </c>
       <c r="G2" s="1">
         <f>E2*22.75*10^-3/39</f>
@@ -1561,8 +1561,8 @@
         <v>178</v>
       </c>
       <c r="I2" s="1">
-        <f>H2*0.2*9.80665</f>
-        <v>349.11673999999999</v>
+        <f>H2*0.2*9.80665*0.8095</f>
+        <v>282.61000102999998</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -1570,12 +1570,12 @@
         <v>40</v>
       </c>
       <c r="B3" s="1">
-        <f>40*0.2*9.80665</f>
-        <v>78.453199999999995</v>
+        <f>0.04*0.2*9.80665*809.5</f>
+        <v>63.5078654</v>
       </c>
       <c r="C3" s="1">
         <f>22.75*10^-3 * 2 / B3 * 10^3 * 2</f>
-        <v>1.1599271922623933</v>
+        <v>1.4328933814235867</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>8</v>
@@ -1583,25 +1583,33 @@
       <c r="E3" s="1">
         <v>112</v>
       </c>
-      <c r="F3" s="1">
-        <f>E3*0.2*9.80665</f>
-        <v>219.66896</v>
+      <c r="F3" s="3">
+        <f t="shared" ref="F3:F6" si="0">E3*0.2*9.80665*0.8095</f>
+        <v>177.82202312000001</v>
       </c>
       <c r="G3" s="1">
-        <f t="shared" ref="G3:G6" si="0">E3*22.75*10^-3/39</f>
+        <f t="shared" ref="G3:G6" si="1">E3*22.75*10^-3/39</f>
         <v>6.533333333333334E-2</v>
       </c>
       <c r="H3" s="1">
         <v>179</v>
       </c>
       <c r="I3" s="1">
-        <f t="shared" ref="I3:I6" si="1">H3*0.2*9.80665</f>
-        <v>351.07807000000003</v>
+        <f t="shared" ref="I3:I6" si="2">H3*0.2*9.80665*0.8095</f>
+        <v>284.19769766500002</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C4">
-        <v>2.1</v>
+      <c r="A4" s="1">
+        <v>40</v>
+      </c>
+      <c r="B4" s="1">
+        <f>0.04*0.2*9.80665*809.5</f>
+        <v>63.5078654</v>
+      </c>
+      <c r="C4" s="1">
+        <f t="shared" ref="C4:C6" si="3">22.75*10^-3 * 2 / B4 * 10^3 * 2</f>
+        <v>1.4328933814235867</v>
       </c>
       <c r="D4" s="4">
         <v>1.45</v>
@@ -1609,63 +1617,88 @@
       <c r="E4" s="1">
         <v>112</v>
       </c>
-      <c r="F4" s="1">
-        <f>E4*0.2*9.80665</f>
-        <v>219.66896</v>
+      <c r="F4" s="3">
+        <f t="shared" si="0"/>
+        <v>177.82202312000001</v>
       </c>
       <c r="G4" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.533333333333334E-2</v>
       </c>
       <c r="H4" s="1">
         <v>181</v>
       </c>
       <c r="I4" s="1">
-        <f t="shared" si="1"/>
-        <v>355.00073000000003</v>
+        <f t="shared" si="2"/>
+        <v>287.37309093500005</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C5">
-        <v>0.65</v>
+      <c r="A5" s="1">
+        <v>41</v>
+      </c>
+      <c r="B5" s="1">
+        <f>0.041*0.2*9.80665*809.5</f>
+        <v>65.095562035</v>
+      </c>
+      <c r="C5" s="1">
+        <f t="shared" si="3"/>
+        <v>1.3979447623644747</v>
+      </c>
+      <c r="D5">
+        <v>2.1</v>
       </c>
       <c r="E5" s="4">
         <v>111</v>
       </c>
-      <c r="F5" s="1">
-        <f>E5*0.2*9.80665</f>
-        <v>217.70763000000002</v>
+      <c r="F5" s="3">
+        <f t="shared" si="0"/>
+        <v>176.23432648500003</v>
       </c>
       <c r="G5" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.4750000000000002E-2</v>
       </c>
       <c r="H5" s="1">
         <v>181</v>
       </c>
       <c r="I5" s="1">
-        <f t="shared" si="1"/>
-        <v>355.00073000000003</v>
+        <f t="shared" si="2"/>
+        <v>287.37309093500005</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>39</v>
+      </c>
+      <c r="B6" s="1">
+        <f t="shared" ref="B6" si="4">0.039*0.2*9.80665*809.5</f>
+        <v>61.920168765</v>
+      </c>
+      <c r="C6" s="1">
+        <f t="shared" si="3"/>
+        <v>1.4696342373575246</v>
+      </c>
+      <c r="D6">
+        <v>0.65</v>
+      </c>
       <c r="E6" s="4">
         <v>112</v>
       </c>
-      <c r="F6" s="4">
-        <f>E6*0.2*9.80665</f>
-        <v>219.66896</v>
+      <c r="F6" s="3">
+        <f t="shared" si="0"/>
+        <v>177.82202312000001</v>
       </c>
       <c r="G6" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.533333333333334E-2</v>
       </c>
       <c r="H6" s="1">
         <v>180</v>
       </c>
       <c r="I6" s="1">
-        <f t="shared" si="1"/>
-        <v>353.0394</v>
+        <f t="shared" si="2"/>
+        <v>285.78539430000001</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -1714,7 +1747,8 @@
         <v>349.11673999999999</v>
       </c>
       <c r="H9" s="1">
-        <v>348.33220799999998</v>
+        <f>348.332208*0.8095</f>
+        <v>281.97492237599999</v>
       </c>
       <c r="I9" s="1">
         <v>25.1</v>
@@ -1740,7 +1774,8 @@
         <v>345.19407999999999</v>
       </c>
       <c r="H10" s="1">
-        <v>346.37087799999995</v>
+        <f>346.370878*0.8095</f>
+        <v>280.38722574100001</v>
       </c>
       <c r="I10" s="1">
         <v>28.1</v>
@@ -1766,7 +1801,8 @@
         <v>347.15540999999996</v>
       </c>
       <c r="H11" s="1">
-        <v>344.40954799999997</v>
+        <f>344.409548*0.8095</f>
+        <v>278.79952910599997</v>
       </c>
       <c r="I11" s="1">
         <v>31</v>
@@ -1792,7 +1828,8 @@
         <v>347.15540999999996</v>
       </c>
       <c r="J12" s="1">
-        <v>346.37087799999989</v>
+        <f>346.370878*0.8095</f>
+        <v>280.38722574100001</v>
       </c>
       <c r="K12" s="1">
         <v>33.9</v>
@@ -1818,7 +1855,8 @@
         <v>343.23275000000001</v>
       </c>
       <c r="H13" s="1">
-        <v>343.23275000000001</v>
+        <f>343.23275*0.8095</f>
+        <v>277.84691112500002</v>
       </c>
       <c r="I13" s="1">
         <v>37</v>
@@ -1849,7 +1887,8 @@
         <v>343.23275000000001</v>
       </c>
       <c r="H14" s="1">
-        <v>342.05595199999999</v>
+        <f>342.055952*0.8095</f>
+        <v>276.89429314400002</v>
       </c>
       <c r="I14" s="1">
         <v>40</v>
@@ -1880,7 +1919,8 @@
         <v>343.23275000000001</v>
       </c>
       <c r="J15" s="1">
-        <v>343.23275000000001</v>
+        <f>343.23275*0.8095</f>
+        <v>277.84691112500002</v>
       </c>
       <c r="K15" s="1">
         <v>43</v>
@@ -1911,7 +1951,8 @@
         <v>341.27141999999998</v>
       </c>
       <c r="H16" s="1">
-        <v>339.31009</v>
+        <f>339.31009*0.8095</f>
+        <v>274.67151785499999</v>
       </c>
       <c r="I16" s="1">
         <v>45.9</v>
@@ -1942,7 +1983,8 @@
         <v>337.34876000000003</v>
       </c>
       <c r="H17" s="1">
-        <v>337.34876000000003</v>
+        <f>337.34876*0.8095</f>
+        <v>273.08382122</v>
       </c>
       <c r="I17" s="1">
         <v>48.9</v>
@@ -1973,7 +2015,8 @@
         <v>339.31009</v>
       </c>
       <c r="J18" s="1">
-        <v>339.31009</v>
+        <f>339.31009*0.8095</f>
+        <v>274.67151785499999</v>
       </c>
       <c r="K18" s="1">
         <v>51.9</v>
@@ -2004,8 +2047,8 @@
         <v>337.34876000000003</v>
       </c>
       <c r="H19" s="1">
-        <f>AVERAGE(B19:F19)</f>
-        <v>336.17196200000001</v>
+        <f>336.171962*0.8095</f>
+        <v>272.131203239</v>
       </c>
       <c r="I19" s="1">
         <v>54.8</v>
@@ -2036,8 +2079,8 @@
         <v>333.42610000000002</v>
       </c>
       <c r="H20" s="1">
-        <f>AVERAGE(B20:F20)</f>
-        <v>334.60289799999998</v>
+        <f>334.602898*0.8095</f>
+        <v>270.86104593099998</v>
       </c>
       <c r="I20" s="1">
         <v>58</v>
@@ -2045,6 +2088,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="C17 D17:E17 F18 C19" formula="1"/>
+  </ignoredErrors>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>